<commit_message>
Updated bus matrix in Dictionaries
Signed-off-by: RojanAsl <aslani.roj@gmail.com>
</commit_message>
<xml_diff>
--- a/Model-designs/Dictionaries.xlsx
+++ b/Model-designs/Dictionaries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmigu\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uporto-my.sharepoint.com/personal/up202204382_up_pt/Documents/22-2/AD/PRJ/Git/DW_project/Model-designs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D7881AF-201F-4CE4-BC64-0B6A91331CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{3D7881AF-201F-4CE4-BC64-0B6A91331CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAFEB35D-E367-4197-B53D-2B68E3619132}"/>
   <bookViews>
-    <workbookView xWindow="4344" yWindow="2004" windowWidth="17280" windowHeight="8880" xr2:uid="{107B6A6F-3B59-46BE-8B41-F06765D6C700}"/>
+    <workbookView xWindow="2505" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{107B6A6F-3B59-46BE-8B41-F06765D6C700}"/>
   </bookViews>
   <sheets>
     <sheet name="Facts" sheetId="3" r:id="rId1"/>
@@ -860,10 +860,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -876,44 +875,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -932,7 +928,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1230,373 +1226,371 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7CB58F-A90E-494D-87A4-EF24C5DA7232}">
   <dimension ref="B2:Q22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="4" t="s">
+    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="K3" s="4" t="s">
+      <c r="H3" s="22"/>
+      <c r="K3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25" t="s">
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="Q3" s="26"/>
-    </row>
-    <row r="4" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="24" t="s">
+      <c r="Q3" s="22"/>
+    </row>
+    <row r="4" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
-      <c r="K4" s="24" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+      <c r="K4" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="L4" s="29"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="31"/>
-    </row>
-    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="23" t="s">
+      <c r="L4" s="23"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="25"/>
+    </row>
+    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
-      <c r="K5" s="23" t="s">
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="30"/>
+      <c r="K5" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="35"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="32" t="s">
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B6" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-      <c r="K6" s="32" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+      <c r="K6" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="L6" s="29"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="31"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="33" t="s">
+      <c r="L6" s="23"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="25"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B7" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-      <c r="K7" s="33" t="s">
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+      <c r="K7" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="L7" s="29"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="31"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="33" t="s">
+      <c r="L7" s="23"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="25"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B8" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-      <c r="K8" s="33" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+      <c r="K8" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="L8" s="36"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="31"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="33" t="s">
+      <c r="L8" s="23"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="25"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B9" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-      <c r="K9" s="33" t="s">
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
+      <c r="K9" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="L9" s="36"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="31"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="33" t="s">
+      <c r="L9" s="23"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="25"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B10" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
-      <c r="K10" s="33" t="s">
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="25"/>
+      <c r="K10" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="L10" s="36"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="31"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="L10" s="23"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="25"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B11" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
-      <c r="K11" s="33" t="s">
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="25"/>
+      <c r="K11" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="L11" s="36"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="31"/>
-    </row>
-    <row r="12" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="33" t="s">
+      <c r="L11" s="23"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="25"/>
+    </row>
+    <row r="12" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="31"/>
-      <c r="K12" s="33" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="25"/>
+      <c r="K12" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="L12" s="36"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="31"/>
-    </row>
-    <row r="13" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="33" t="s">
+      <c r="L12" s="23"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="25"/>
+    </row>
+    <row r="13" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="28"/>
-      <c r="K13" s="23" t="s">
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="25"/>
+      <c r="K13" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="33" t="s">
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B14" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
-      <c r="K14" s="33" t="s">
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+      <c r="K14" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="L14" s="36" t="s">
+      <c r="L14" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="31"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="33" t="s">
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="25"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B15" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-      <c r="K15" s="33" t="s">
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="25"/>
+      <c r="K15" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="L15" s="36" t="s">
+      <c r="L15" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="31"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="33" t="s">
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="25"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B16" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="33" t="s">
+      <c r="C16" s="23"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="33" t="s">
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="31"/>
-    </row>
-    <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="23" t="s">
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="25"/>
+    </row>
+    <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="28"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="33" t="s">
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="31"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="33" t="s">
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="25"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="31"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="33" t="s">
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="25"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="31"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1614,333 +1608,333 @@
   <dimension ref="B2:AR16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H16"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" customWidth="1"/>
+    <col min="11" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="4" t="s">
+    <row r="2" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="K3" s="4" t="s">
+      <c r="H3" s="5"/>
+      <c r="K3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5" t="s">
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="6"/>
-      <c r="T3" s="4" t="s">
+      <c r="Q3" s="5"/>
+      <c r="T3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5" t="s">
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Z3" s="6"/>
-      <c r="AC3" s="4" t="s">
+      <c r="Z3" s="5"/>
+      <c r="AC3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AD3" s="5" t="s">
+      <c r="AD3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AE3" s="5" t="s">
+      <c r="AE3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AF3" s="5"/>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="5" t="s">
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AI3" s="6"/>
-      <c r="AL3" s="4" t="s">
+      <c r="AI3" s="5"/>
+      <c r="AL3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AM3" s="5" t="s">
+      <c r="AM3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AN3" s="5" t="s">
+      <c r="AN3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AO3" s="5"/>
-      <c r="AP3" s="5"/>
-      <c r="AQ3" s="5" t="s">
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AR3" s="6"/>
-    </row>
-    <row r="4" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
+      <c r="AR3" s="5"/>
+    </row>
+    <row r="4" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="9"/>
-      <c r="K4" s="8" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="8"/>
+      <c r="K4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7" t="s">
+      <c r="L4" s="6"/>
+      <c r="M4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="9"/>
-      <c r="T4" s="8" t="s">
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="8"/>
+      <c r="T4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7" t="s">
+      <c r="U4" s="6"/>
+      <c r="V4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="9"/>
-      <c r="AC4" s="8" t="s">
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="8"/>
+      <c r="AC4" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="7" t="s">
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AF4" s="7"/>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="7"/>
-      <c r="AI4" s="9"/>
-      <c r="AL4" s="8" t="s">
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="8"/>
+      <c r="AL4" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="AM4" s="7"/>
-      <c r="AN4" s="7" t="s">
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="7"/>
-      <c r="AQ4" s="7"/>
-      <c r="AR4" s="9"/>
-    </row>
-    <row r="5" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="4" t="s">
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
+      <c r="AR4" s="8"/>
+    </row>
+    <row r="5" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="K5" s="4" t="s">
+      <c r="H5" s="5"/>
+      <c r="K5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="6"/>
-      <c r="T5" s="4" t="s">
+      <c r="Q5" s="5"/>
+      <c r="T5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="V5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="W5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="X5" s="5" t="s">
+      <c r="X5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Y5" s="5" t="s">
+      <c r="Y5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Z5" s="6"/>
-      <c r="AC5" s="4" t="s">
+      <c r="Z5" s="5"/>
+      <c r="AC5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AD5" s="5" t="s">
+      <c r="AD5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AE5" s="5" t="s">
+      <c r="AE5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AF5" s="5" t="s">
+      <c r="AF5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AG5" s="5" t="s">
+      <c r="AG5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AH5" s="5" t="s">
+      <c r="AH5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AI5" s="6"/>
-      <c r="AL5" s="4" t="s">
+      <c r="AI5" s="5"/>
+      <c r="AL5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AM5" s="5" t="s">
+      <c r="AM5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AN5" s="5" t="s">
+      <c r="AN5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AO5" s="5" t="s">
+      <c r="AO5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AP5" s="5" t="s">
+      <c r="AP5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AQ5" s="5" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AR5" s="6"/>
-    </row>
-    <row r="6" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+      <c r="AR5" s="5"/>
+    </row>
+    <row r="6" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="B6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="11"/>
-      <c r="K6" s="10" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="10"/>
+      <c r="K6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3" t="s">
+      <c r="M6" s="2"/>
+      <c r="N6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="11"/>
-      <c r="T6" s="10" t="s">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="10"/>
+      <c r="T6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="U6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3" t="s">
+      <c r="V6" s="2"/>
+      <c r="W6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="X6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="11"/>
-      <c r="AC6" s="10" t="s">
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="10"/>
+      <c r="AC6" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AD6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3" t="s">
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="AG6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="11"/>
-      <c r="AL6" s="10" t="s">
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="10"/>
+      <c r="AL6" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="AM6" s="3" t="s">
+      <c r="AM6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AN6" s="3"/>
-      <c r="AO6" s="3" t="s">
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="AP6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AQ6" s="3"/>
-      <c r="AR6" s="11"/>
-    </row>
-    <row r="7" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B7" s="12" t="s">
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="10"/>
+    </row>
+    <row r="7" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="B7" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1956,22 +1950,22 @@
         <v>31</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="13"/>
-      <c r="K7" s="10" t="s">
+      <c r="H7" s="12"/>
+      <c r="K7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M7" s="3"/>
+      <c r="M7" s="2"/>
       <c r="O7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="2">
         <v>64</v>
       </c>
-      <c r="Q7" s="11"/>
-      <c r="T7" s="12" t="s">
+      <c r="Q7" s="10"/>
+      <c r="T7" s="11" t="s">
         <v>66</v>
       </c>
       <c r="U7" s="1" t="s">
@@ -1987,8 +1981,8 @@
       <c r="Y7" s="1">
         <v>32</v>
       </c>
-      <c r="Z7" s="13"/>
-      <c r="AC7" s="12" t="s">
+      <c r="Z7" s="12"/>
+      <c r="AC7" s="11" t="s">
         <v>103</v>
       </c>
       <c r="AD7" s="1"/>
@@ -2000,12 +1994,12 @@
       <c r="AH7" s="1">
         <v>2</v>
       </c>
-      <c r="AI7" s="13"/>
-      <c r="AL7" s="12" t="s">
+      <c r="AI7" s="12"/>
+      <c r="AL7" s="11" t="s">
         <v>110</v>
       </c>
       <c r="AM7" s="1"/>
-      <c r="AN7" s="12" t="s">
+      <c r="AN7" s="11" t="s">
         <v>111</v>
       </c>
       <c r="AO7" s="1" t="s">
@@ -2015,13 +2009,13 @@
         <v>31</v>
       </c>
       <c r="AQ7" s="1"/>
-      <c r="AR7" s="13"/>
-    </row>
-    <row r="8" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
+      <c r="AR7" s="12"/>
+    </row>
+    <row r="8" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -2036,8 +2030,8 @@
       <c r="G8" s="1">
         <v>32</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="K8" s="12" t="s">
+      <c r="H8" s="12"/>
+      <c r="K8" s="11" t="s">
         <v>49</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -2051,11 +2045,11 @@
       <c r="P8" s="1">
         <v>32</v>
       </c>
-      <c r="Q8" s="13"/>
-      <c r="T8" s="12" t="s">
+      <c r="Q8" s="12"/>
+      <c r="T8" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="U8" s="1" t="s">
         <v>75</v>
       </c>
       <c r="V8" s="1"/>
@@ -2068,11 +2062,11 @@
       <c r="Y8" s="1">
         <v>32</v>
       </c>
-      <c r="Z8" s="13"/>
-      <c r="AC8" s="12" t="s">
+      <c r="Z8" s="12"/>
+      <c r="AC8" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="AD8" s="2"/>
+      <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1" t="s">
@@ -2081,12 +2075,12 @@
       <c r="AH8" s="1">
         <v>2</v>
       </c>
-      <c r="AI8" s="13"/>
-      <c r="AL8" s="12" t="s">
+      <c r="AI8" s="12"/>
+      <c r="AL8" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="AM8" s="2"/>
-      <c r="AN8" s="12" t="s">
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="11" t="s">
         <v>111</v>
       </c>
       <c r="AO8" s="1" t="s">
@@ -2098,13 +2092,13 @@
       <c r="AQ8" s="1">
         <v>2</v>
       </c>
-      <c r="AR8" s="13"/>
-    </row>
-    <row r="9" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
+      <c r="AR8" s="12"/>
+    </row>
+    <row r="9" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -2117,11 +2111,11 @@
         <v>31</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="13"/>
-      <c r="K9" s="12" t="s">
+      <c r="H9" s="12"/>
+      <c r="K9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="1" t="s">
         <v>50</v>
       </c>
       <c r="M9" s="1"/>
@@ -2132,11 +2126,11 @@
       <c r="P9" s="1">
         <v>32</v>
       </c>
-      <c r="Q9" s="13"/>
-      <c r="T9" s="12" t="s">
+      <c r="Q9" s="12"/>
+      <c r="T9" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="U9" s="1" t="s">
         <v>95</v>
       </c>
       <c r="V9" s="1"/>
@@ -2149,11 +2143,11 @@
       <c r="Y9" s="1">
         <v>256</v>
       </c>
-      <c r="Z9" s="13"/>
-      <c r="AC9" s="12" t="s">
+      <c r="Z9" s="12"/>
+      <c r="AC9" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="AD9" s="2"/>
+      <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1" t="s">
@@ -2162,12 +2156,12 @@
       <c r="AH9" s="1">
         <v>2</v>
       </c>
-      <c r="AI9" s="13"/>
-      <c r="AL9" s="12" t="s">
+      <c r="AI9" s="12"/>
+      <c r="AL9" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="AM9" s="2"/>
-      <c r="AN9" s="12" t="s">
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="11" t="s">
         <v>106</v>
       </c>
       <c r="AO9" s="1" t="s">
@@ -2177,13 +2171,13 @@
         <v>31</v>
       </c>
       <c r="AQ9" s="1"/>
-      <c r="AR9" s="13"/>
-    </row>
-    <row r="10" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
+      <c r="AR9" s="12"/>
+    </row>
+    <row r="10" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -2198,11 +2192,11 @@
       <c r="G10" s="1">
         <v>32</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="K10" s="12" t="s">
+      <c r="H10" s="12"/>
+      <c r="K10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="M10" s="1"/>
@@ -2213,11 +2207,11 @@
       <c r="P10" s="1">
         <v>32</v>
       </c>
-      <c r="Q10" s="13"/>
-      <c r="T10" s="12" t="s">
+      <c r="Q10" s="12"/>
+      <c r="T10" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="U10" s="1" t="s">
         <v>96</v>
       </c>
       <c r="V10" s="1"/>
@@ -2230,11 +2224,11 @@
       <c r="Y10" s="1">
         <v>8</v>
       </c>
-      <c r="Z10" s="13"/>
-      <c r="AC10" s="12" t="s">
+      <c r="Z10" s="12"/>
+      <c r="AC10" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="AD10" s="2"/>
+      <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
       <c r="AG10" s="1" t="s">
@@ -2243,12 +2237,12 @@
       <c r="AH10" s="1">
         <v>2</v>
       </c>
-      <c r="AI10" s="13"/>
-      <c r="AL10" s="12" t="s">
+      <c r="AI10" s="12"/>
+      <c r="AL10" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="AM10" s="2"/>
-      <c r="AN10" s="12" t="s">
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="11" t="s">
         <v>106</v>
       </c>
       <c r="AO10" s="1" t="s">
@@ -2260,13 +2254,13 @@
       <c r="AQ10" s="1">
         <v>2</v>
       </c>
-      <c r="AR10" s="13"/>
-    </row>
-    <row r="11" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
+      <c r="AR10" s="12"/>
+    </row>
+    <row r="11" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="B11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2279,11 +2273,11 @@
         <v>31</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="13"/>
-      <c r="K11" s="12" t="s">
+      <c r="H11" s="12"/>
+      <c r="K11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="1" t="s">
         <v>62</v>
       </c>
       <c r="M11" s="1"/>
@@ -2294,11 +2288,11 @@
       <c r="P11" s="1">
         <v>32</v>
       </c>
-      <c r="Q11" s="13"/>
-      <c r="T11" s="12" t="s">
+      <c r="Q11" s="12"/>
+      <c r="T11" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="U11" s="1" t="s">
         <v>97</v>
       </c>
       <c r="V11" s="1"/>
@@ -2311,11 +2305,11 @@
       <c r="Y11" s="1">
         <v>32</v>
       </c>
-      <c r="Z11" s="13"/>
-      <c r="AC11" s="12" t="s">
+      <c r="Z11" s="12"/>
+      <c r="AC11" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="AD11" s="2"/>
+      <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1" t="s">
@@ -2324,12 +2318,12 @@
       <c r="AH11" s="1">
         <v>4</v>
       </c>
-      <c r="AI11" s="13"/>
-      <c r="AL11" s="12" t="s">
+      <c r="AI11" s="12"/>
+      <c r="AL11" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AM11" s="2"/>
-      <c r="AN11" s="12" t="s">
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="11" t="s">
         <v>115</v>
       </c>
       <c r="AO11" s="1" t="s">
@@ -2339,13 +2333,13 @@
         <v>31</v>
       </c>
       <c r="AQ11" s="1"/>
-      <c r="AR11" s="13"/>
-    </row>
-    <row r="12" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B12" s="12" t="s">
+      <c r="AR11" s="12"/>
+    </row>
+    <row r="12" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="B12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -2360,11 +2354,11 @@
       <c r="G12" s="1">
         <v>32</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="K12" s="12" t="s">
+      <c r="H12" s="12"/>
+      <c r="K12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="1" t="s">
         <v>63</v>
       </c>
       <c r="M12" s="1"/>
@@ -2373,11 +2367,11 @@
         <v>57</v>
       </c>
       <c r="P12" s="1"/>
-      <c r="Q12" s="13"/>
-      <c r="T12" s="12" t="s">
+      <c r="Q12" s="12"/>
+      <c r="T12" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="U12" s="1" t="s">
         <v>98</v>
       </c>
       <c r="V12" s="1" t="s">
@@ -2390,12 +2384,12 @@
         <v>31</v>
       </c>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="13"/>
-      <c r="AL12" s="12" t="s">
+      <c r="Z12" s="12"/>
+      <c r="AL12" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AM12" s="2"/>
-      <c r="AN12" s="12" t="s">
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="11" t="s">
         <v>115</v>
       </c>
       <c r="AO12" s="1" t="s">
@@ -2407,13 +2401,13 @@
       <c r="AQ12" s="1">
         <v>2</v>
       </c>
-      <c r="AR12" s="13"/>
-    </row>
-    <row r="13" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B13" s="12" t="s">
+      <c r="AR12" s="12"/>
+    </row>
+    <row r="13" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="B13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2426,11 +2420,11 @@
         <v>31</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="13"/>
-      <c r="K13" s="12" t="s">
+      <c r="H13" s="12"/>
+      <c r="K13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="1" t="s">
         <v>64</v>
       </c>
       <c r="M13" s="1"/>
@@ -2438,14 +2432,14 @@
       <c r="O13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="P13" s="18">
+      <c r="P13" s="16">
         <v>15</v>
       </c>
-      <c r="Q13" s="13"/>
-      <c r="T13" s="12" t="s">
+      <c r="Q13" s="12"/>
+      <c r="T13" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="U13" s="1" t="s">
         <v>99</v>
       </c>
       <c r="V13" s="1" t="s">
@@ -2460,12 +2454,12 @@
       <c r="Y13" s="1">
         <v>32</v>
       </c>
-      <c r="Z13" s="13"/>
-      <c r="AL13" s="12" t="s">
+      <c r="Z13" s="12"/>
+      <c r="AL13" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="AM13" s="2"/>
-      <c r="AN13" s="12" t="s">
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="11" t="s">
         <v>116</v>
       </c>
       <c r="AO13" s="1" t="s">
@@ -2475,13 +2469,13 @@
         <v>31</v>
       </c>
       <c r="AQ13" s="1"/>
-      <c r="AR13" s="13"/>
-    </row>
-    <row r="14" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B14" s="12" t="s">
+      <c r="AR13" s="12"/>
+    </row>
+    <row r="14" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -2496,11 +2490,11 @@
       <c r="G14" s="1">
         <v>32</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="K14" s="12" t="s">
+      <c r="H14" s="12"/>
+      <c r="K14" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="1" t="s">
         <v>65</v>
       </c>
       <c r="M14" s="1"/>
@@ -2508,14 +2502,14 @@
       <c r="O14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="P14" s="18">
+      <c r="P14" s="16">
         <v>15</v>
       </c>
-      <c r="Q14" s="13"/>
-      <c r="T14" s="12" t="s">
+      <c r="Q14" s="12"/>
+      <c r="T14" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="U14" s="2" t="s">
+      <c r="U14" s="1" t="s">
         <v>100</v>
       </c>
       <c r="V14" s="1" t="s">
@@ -2528,12 +2522,12 @@
         <v>31</v>
       </c>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="13"/>
-      <c r="AL14" s="12" t="s">
+      <c r="Z14" s="12"/>
+      <c r="AL14" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AM14" s="2"/>
-      <c r="AN14" s="12" t="s">
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="11" t="s">
         <v>116</v>
       </c>
       <c r="AO14" s="1" t="s">
@@ -2545,13 +2539,13 @@
       <c r="AQ14" s="1">
         <v>2</v>
       </c>
-      <c r="AR14" s="13"/>
-    </row>
-    <row r="15" spans="2:44" x14ac:dyDescent="0.3">
-      <c r="B15" s="12" t="s">
+      <c r="AR14" s="12"/>
+    </row>
+    <row r="15" spans="2:44" x14ac:dyDescent="0.35">
+      <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2564,11 +2558,11 @@
         <v>31</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="13"/>
-      <c r="K15" s="12" t="s">
+      <c r="H15" s="12"/>
+      <c r="K15" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="1" t="s">
         <v>90</v>
       </c>
       <c r="M15" s="1" t="s">
@@ -2581,11 +2575,11 @@
         <v>31</v>
       </c>
       <c r="P15" s="1"/>
-      <c r="Q15" s="13"/>
-      <c r="T15" s="2" t="s">
+      <c r="Q15" s="12"/>
+      <c r="T15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="U15" s="2" t="s">
+      <c r="U15" s="1" t="s">
         <v>101</v>
       </c>
       <c r="V15" s="1" t="s">
@@ -2600,12 +2594,12 @@
       <c r="Y15" s="1">
         <v>32</v>
       </c>
-      <c r="Z15" s="13"/>
-      <c r="AL15" s="12" t="s">
+      <c r="Z15" s="12"/>
+      <c r="AL15" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="AM15" s="2"/>
-      <c r="AN15" s="12" t="s">
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="11" t="s">
         <v>107</v>
       </c>
       <c r="AO15" s="1" t="s">
@@ -2617,38 +2611,38 @@
       <c r="AQ15" s="1">
         <v>4</v>
       </c>
-      <c r="AR15" s="13"/>
-    </row>
-    <row r="16" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="14" t="s">
+      <c r="AR15" s="12"/>
+    </row>
+    <row r="16" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="14" t="s">
         <v>32</v>
       </c>
       <c r="G16" s="1">
         <v>32</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="K16" s="12" t="s">
+      <c r="H16" s="15"/>
+      <c r="K16" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="1" t="s">
         <v>51</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N16" s="16" t="s">
+      <c r="N16" s="14" t="s">
         <v>34</v>
       </c>
       <c r="O16" s="1" t="s">
@@ -2657,7 +2651,7 @@
       <c r="P16" s="1">
         <v>320</v>
       </c>
-      <c r="Q16" s="13"/>
+      <c r="Q16" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2666,29 +2660,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49019117-B635-48EC-85BA-78E6FF0E2E6B}">
-  <dimension ref="B3:I7"/>
+  <dimension ref="B3:H7"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="5.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="5.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E3" s="19" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="E3" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" spans="2:9" ht="116.4" x14ac:dyDescent="0.3">
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+    </row>
+    <row r="4" spans="2:8" ht="117" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>76</v>
       </c>
@@ -2698,83 +2691,79 @@
       <c r="D4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="22" t="s">
+      <c r="F4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="G4" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="H4" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="21" t="s">
+    <row r="5" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20" t="s">
+      <c r="F5" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+    <row r="6" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7" spans="2:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="21" t="s">
+      <c r="H6" s="17"/>
+    </row>
+    <row r="7" spans="2:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20" t="s">
+      <c r="E7" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="F7" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20" t="s">
+      <c r="G7" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>